<commit_message>
"Refactorizo paths archivos del cliente"
</commit_message>
<xml_diff>
--- a/Template Reporte.xlsx
+++ b/Template Reporte.xlsx
@@ -1,58 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Documents\extraccion_de_datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcos.tulli.sp\Documents\extraccion_de_datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CA6C12-E933-49E3-8033-96EB58458F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{22226BF8-EC60-4980-86A7-D16BB6A07081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{B5009FDF-F9ED-4BE2-B3E3-26D42E521AB8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Reporte" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Web site</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>https://www.ambito.com/contenidos/dolar-cl.html</t>
-  </si>
-  <si>
-    <t>https://www.cac.bcr.com.ar/es/precios-de-pizarra/consultas</t>
-  </si>
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>BCR</t>
-  </si>
-  <si>
-    <t>Lascombes S.A.</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,35 +44,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="2"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -100,17 +62,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -127,7 +85,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -143,7 +101,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -155,7 +113,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -172,7 +130,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -202,12 +160,29 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -237,6 +212,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -388,53 +380,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CADC6BCF-AE9B-4152-8B72-358A05A88C53}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="28.26953125" customWidth="1"/>
-    <col min="2" max="2" width="56.453125" customWidth="1"/>
-    <col min="3" max="3" width="64.54296875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{2134AF76-E927-43D4-B118-7C716F1B2F7C}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{E993DEFC-A041-4520-B445-8DEFAA6F72DA}"/>
-  </hyperlinks>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>